<commit_message>
excel, update if found
</commit_message>
<xml_diff>
--- a/Excel_Sample_Lookup_Prototype-2.xlsx
+++ b/Excel_Sample_Lookup_Prototype-2.xlsx
@@ -1,20 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/suhail/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\SearchWebsite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BFEB7B2-607B-094F-9893-8780C205E79B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6420" yWindow="3120" windowWidth="16820" windowHeight="11260" xr2:uid="{A4C194D6-772E-1942-B97B-722E1834D30C}"/>
+    <workbookView xWindow="6420" yWindow="3120" windowWidth="16815" windowHeight="11265"/>
   </bookViews>
   <sheets>
-    <sheet name="Front End" sheetId="2" r:id="rId1"/>
-    <sheet name="Back End" sheetId="1" r:id="rId2"/>
+    <sheet name="Back End" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,62 +23,8 @@
 </workbook>
 </file>
 
-<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
-  <authors>
-    <author>Microsoft Office User</author>
-  </authors>
-  <commentList>
-    <comment ref="C5" authorId="0" shapeId="0" xr:uid="{D18605AD-FEA5-244C-A594-C9EB1B6594F7}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">121smith
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">122smith
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">123smith
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">etc will show corresponding URLs from the backend table.
-</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>link</t>
   </si>
@@ -113,28 +57,13 @@
   </si>
   <si>
     <t>https://www.URLforUser3.com</t>
-  </si>
-  <si>
-    <t>CLICK &gt;&gt;</t>
-  </si>
-  <si>
-    <t>Welcome to the survey.</t>
-  </si>
-  <si>
-    <t>&lt;&lt; CLICK</t>
-  </si>
-  <si>
-    <t>GO</t>
-  </si>
-  <si>
-    <t>Please enter the ID you were told to use and click the "Go" button</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,62 +85,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -219,51 +102,15 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -578,78 +425,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F7832B17-D748-2346-BF23-1A7D88D5CB06}">
-  <dimension ref="A2:E8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="4.1640625" customWidth="1"/>
-    <col min="3" max="3" width="54.83203125" customWidth="1"/>
-    <col min="4" max="4" width="4.5" style="10" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C2" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="9"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C3" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D3" s="9"/>
-    </row>
-    <row r="4" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="A8" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="4" t="str">
-        <f>VLOOKUP(C5,'Back End'!A:C,3,0)</f>
-        <v>https://www.URLforUser1.com</v>
-      </c>
-      <c r="D8" s="12"/>
-      <c r="E8" s="13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00BB05C5-87AE-5D46-81A8-DFBB6B65F5C4}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.1640625" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" customWidth="1"/>
+    <col min="2" max="2" width="21.125" customWidth="1"/>
+    <col min="3" max="3" width="23.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>8</v>
       </c>
@@ -660,7 +449,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -671,7 +460,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,7 +471,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -695,9 +484,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{CA8B745C-A09C-F54B-B34A-88BF9A2E0B10}"/>
-    <hyperlink ref="C3" r:id="rId2" xr:uid="{56A0502A-B1D4-624A-BA46-9BF5D0CAF704}"/>
-    <hyperlink ref="C4" r:id="rId3" xr:uid="{8422B589-BE1F-F74F-8E86-0248839746F7}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3" r:id="rId2"/>
+    <hyperlink ref="C4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>